<commit_message>
Dom g drive (#5)
* remove ptox-metadata-lfs as submodule

* adding submodule support for external repo holdind metadatafiles

* migrated to googledrive
</commit_message>
<xml_diff>
--- a/tests/data/excel/test.xlsx
+++ b/tests/data/excel/test.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R2"/>
+  <dimension ref="A1:S2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -434,99 +434,101 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
+      <c r="B1" s="1" t="inlineStr">
         <is>
           <t>Shipment identifier</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>Label tube / identifier</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>Box No.</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>FreezerBoxID [SENDER TO ADD LABEL TO BOX]</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>Sample position in box</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>Mass including tube (mg)</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>Mass excluding tube (mg)</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>Additional Information</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>partner</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>organism</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>exposure batch</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>replicates for exposure</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>replicates for control</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="O1" s="1" t="inlineStr">
         <is>
           <t>replicates blanks</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
+      <c r="P1" s="1" t="inlineStr">
         <is>
           <t>start date</t>
         </is>
       </c>
-      <c r="P1" s="1" t="inlineStr">
+      <c r="Q1" s="1" t="inlineStr">
         <is>
           <t>end date</t>
         </is>
       </c>
-      <c r="Q1" s="1" t="inlineStr">
+      <c r="R1" s="1" t="inlineStr">
         <is>
           <t>chemical name</t>
         </is>
       </c>
-      <c r="R1" s="1" t="inlineStr">
+      <c r="S1" s="1" t="inlineStr">
         <is>
           <t>dose</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr"/>
+      <c r="A2" s="1" t="n">
+        <v>0</v>
+      </c>
       <c r="B2" t="inlineStr"/>
       <c r="C2" t="inlineStr"/>
       <c r="D2" t="inlineStr"/>
@@ -534,46 +536,47 @@
       <c r="F2" t="inlineStr"/>
       <c r="G2" t="inlineStr"/>
       <c r="H2" t="inlineStr"/>
-      <c r="I2" t="inlineStr">
+      <c r="I2" t="inlineStr"/>
+      <c r="J2" t="inlineStr">
         <is>
           <t>KIT</t>
         </is>
       </c>
-      <c r="J2" t="inlineStr">
+      <c r="K2" t="inlineStr">
         <is>
           <t>organism1</t>
         </is>
       </c>
-      <c r="K2" t="inlineStr">
+      <c r="L2" t="inlineStr">
         <is>
           <t>AA</t>
         </is>
-      </c>
-      <c r="L2" t="n">
-        <v>4</v>
       </c>
       <c r="M2" t="n">
         <v>4</v>
       </c>
       <c r="N2" t="n">
+        <v>4</v>
+      </c>
+      <c r="O2" t="n">
         <v>2</v>
       </c>
-      <c r="O2" t="inlineStr">
+      <c r="P2" t="inlineStr">
         <is>
           <t>2018-01-01</t>
         </is>
       </c>
-      <c r="P2" t="inlineStr">
+      <c r="Q2" t="inlineStr">
         <is>
           <t>2019-01-02</t>
         </is>
       </c>
-      <c r="Q2" t="inlineStr">
+      <c r="R2" t="inlineStr">
         <is>
           <t>chemical1</t>
         </is>
       </c>
-      <c r="R2" t="inlineStr">
+      <c r="S2" t="inlineStr">
         <is>
           <t>0</t>
         </is>

</xml_diff>

<commit_message>
Dom g drive (#6)
* more google drive features
</commit_message>
<xml_diff>
--- a/tests/data/excel/test.xlsx
+++ b/tests/data/excel/test.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:S2"/>
+  <dimension ref="A1:R2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -434,101 +434,99 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Shipment identifier</t>
+        </is>
+      </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Shipment identifier</t>
+          <t>Label tube / identifier</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Label tube / identifier</t>
+          <t>Box No.</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>Box No.</t>
+          <t>FreezerBoxID [SENDER TO ADD LABEL TO BOX]</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>FreezerBoxID [SENDER TO ADD LABEL TO BOX]</t>
+          <t>Sample position in box</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>Sample position in box</t>
+          <t>Mass including tube (mg)</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>Mass including tube (mg)</t>
+          <t>Mass excluding tube (mg)</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>Mass excluding tube (mg)</t>
+          <t>Additional Information</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>Additional Information</t>
+          <t>partner</t>
         </is>
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
-          <t>partner</t>
+          <t>organism</t>
         </is>
       </c>
       <c r="K1" s="1" t="inlineStr">
         <is>
-          <t>organism</t>
+          <t>exposure batch</t>
         </is>
       </c>
       <c r="L1" s="1" t="inlineStr">
         <is>
-          <t>exposure batch</t>
+          <t>replicates for exposure</t>
         </is>
       </c>
       <c r="M1" s="1" t="inlineStr">
         <is>
-          <t>replicates for exposure</t>
+          <t>replicates for control</t>
         </is>
       </c>
       <c r="N1" s="1" t="inlineStr">
         <is>
-          <t>replicates for control</t>
+          <t>replicates blanks</t>
         </is>
       </c>
       <c r="O1" s="1" t="inlineStr">
         <is>
-          <t>replicates blanks</t>
+          <t>start date</t>
         </is>
       </c>
       <c r="P1" s="1" t="inlineStr">
         <is>
-          <t>start date</t>
+          <t>end date</t>
         </is>
       </c>
       <c r="Q1" s="1" t="inlineStr">
         <is>
-          <t>end date</t>
+          <t>chemical name</t>
         </is>
       </c>
       <c r="R1" s="1" t="inlineStr">
-        <is>
-          <t>chemical name</t>
-        </is>
-      </c>
-      <c r="S1" s="1" t="inlineStr">
         <is>
           <t>dose</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="n">
-        <v>0</v>
-      </c>
+      <c r="A2" t="inlineStr"/>
       <c r="B2" t="inlineStr"/>
       <c r="C2" t="inlineStr"/>
       <c r="D2" t="inlineStr"/>
@@ -536,47 +534,46 @@
       <c r="F2" t="inlineStr"/>
       <c r="G2" t="inlineStr"/>
       <c r="H2" t="inlineStr"/>
-      <c r="I2" t="inlineStr"/>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>KIT</t>
+        </is>
+      </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>KIT</t>
+          <t>organism1</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>organism1</t>
-        </is>
-      </c>
-      <c r="L2" t="inlineStr">
-        <is>
           <t>AA</t>
         </is>
+      </c>
+      <c r="L2" t="n">
+        <v>4</v>
       </c>
       <c r="M2" t="n">
         <v>4</v>
       </c>
       <c r="N2" t="n">
-        <v>4</v>
-      </c>
-      <c r="O2" t="n">
         <v>2</v>
       </c>
+      <c r="O2" t="inlineStr">
+        <is>
+          <t>2018-01-01</t>
+        </is>
+      </c>
       <c r="P2" t="inlineStr">
         <is>
-          <t>2018-01-01</t>
+          <t>2019-01-02</t>
         </is>
       </c>
       <c r="Q2" t="inlineStr">
         <is>
-          <t>2019-01-02</t>
+          <t>chemical1</t>
         </is>
       </c>
       <c r="R2" t="inlineStr">
-        <is>
-          <t>chemical1</t>
-        </is>
-      </c>
-      <c r="S2" t="inlineStr">
         <is>
           <t>0</t>
         </is>

</xml_diff>

<commit_message>
Added a small SQLITE DB to handle users
</commit_message>
<xml_diff>
--- a/tests/data/excel/test.xlsx
+++ b/tests/data/excel/test.xlsx
@@ -515,7 +515,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K5"/>
+  <dimension ref="A1:L5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -577,6 +577,11 @@
       <c r="K1" s="1" t="inlineStr">
         <is>
           <t>dose</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>time point</t>
         </is>
       </c>
     </row>
@@ -602,6 +607,11 @@
           <t>0</t>
         </is>
       </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>TP1</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr"/>
@@ -625,6 +635,11 @@
           <t>0</t>
         </is>
       </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>TP1</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr"/>
@@ -648,6 +663,11 @@
           <t>0</t>
         </is>
       </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>TP1</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr"/>
@@ -671,6 +691,11 @@
           <t>0</t>
         </is>
       </c>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t>TP1</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
added a small API + extended tests
</commit_message>
<xml_diff>
--- a/tests/data/excel/test.xlsx
+++ b/tests/data/excel/test.xlsx
@@ -8,7 +8,7 @@
   </bookViews>
   <sheets>
     <sheet name="General Information" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="SAMPLE_TEST" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Exposure conditions" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -515,7 +515,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L5"/>
+  <dimension ref="A1:L11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -697,6 +697,166 @@
         </is>
       </c>
     </row>
+    <row r="6">
+      <c r="A6" t="inlineStr"/>
+      <c r="B6" t="inlineStr"/>
+      <c r="C6" t="inlineStr"/>
+      <c r="D6" t="inlineStr"/>
+      <c r="E6" t="inlineStr"/>
+      <c r="F6" t="inlineStr"/>
+      <c r="G6" t="inlineStr"/>
+      <c r="H6" t="inlineStr"/>
+      <c r="I6" t="n">
+        <v>1</v>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>CONTROL (SEE VEHICLE)</t>
+        </is>
+      </c>
+      <c r="K6" t="n">
+        <v>0</v>
+      </c>
+      <c r="L6" t="inlineStr">
+        <is>
+          <t>TP1</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr"/>
+      <c r="B7" t="inlineStr"/>
+      <c r="C7" t="inlineStr"/>
+      <c r="D7" t="inlineStr"/>
+      <c r="E7" t="inlineStr"/>
+      <c r="F7" t="inlineStr"/>
+      <c r="G7" t="inlineStr"/>
+      <c r="H7" t="inlineStr"/>
+      <c r="I7" t="n">
+        <v>2</v>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>CONTROL (SEE VEHICLE)</t>
+        </is>
+      </c>
+      <c r="K7" t="n">
+        <v>0</v>
+      </c>
+      <c r="L7" t="inlineStr">
+        <is>
+          <t>TP1</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr"/>
+      <c r="B8" t="inlineStr"/>
+      <c r="C8" t="inlineStr"/>
+      <c r="D8" t="inlineStr"/>
+      <c r="E8" t="inlineStr"/>
+      <c r="F8" t="inlineStr"/>
+      <c r="G8" t="inlineStr"/>
+      <c r="H8" t="inlineStr"/>
+      <c r="I8" t="n">
+        <v>3</v>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>CONTROL (SEE VEHICLE)</t>
+        </is>
+      </c>
+      <c r="K8" t="n">
+        <v>0</v>
+      </c>
+      <c r="L8" t="inlineStr">
+        <is>
+          <t>TP1</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr"/>
+      <c r="B9" t="inlineStr"/>
+      <c r="C9" t="inlineStr"/>
+      <c r="D9" t="inlineStr"/>
+      <c r="E9" t="inlineStr"/>
+      <c r="F9" t="inlineStr"/>
+      <c r="G9" t="inlineStr"/>
+      <c r="H9" t="inlineStr"/>
+      <c r="I9" t="n">
+        <v>4</v>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>CONTROL (SEE VEHICLE)</t>
+        </is>
+      </c>
+      <c r="K9" t="n">
+        <v>0</v>
+      </c>
+      <c r="L9" t="inlineStr">
+        <is>
+          <t>TP1</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr"/>
+      <c r="B10" t="inlineStr"/>
+      <c r="C10" t="inlineStr"/>
+      <c r="D10" t="inlineStr"/>
+      <c r="E10" t="inlineStr"/>
+      <c r="F10" t="inlineStr"/>
+      <c r="G10" t="inlineStr"/>
+      <c r="H10" t="inlineStr"/>
+      <c r="I10" t="n">
+        <v>0</v>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>EXTRACTION BLANK</t>
+        </is>
+      </c>
+      <c r="K10" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="L10" t="inlineStr">
+        <is>
+          <t>TP0</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr"/>
+      <c r="B11" t="inlineStr"/>
+      <c r="C11" t="inlineStr"/>
+      <c r="D11" t="inlineStr"/>
+      <c r="E11" t="inlineStr"/>
+      <c r="F11" t="inlineStr"/>
+      <c r="G11" t="inlineStr"/>
+      <c r="H11" t="inlineStr"/>
+      <c r="I11" t="n">
+        <v>0</v>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>EXTRACTION BLANK</t>
+        </is>
+      </c>
+      <c r="K11" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="L11" t="inlineStr">
+        <is>
+          <t>TP0</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
added arrays chemicals_name and single dose per chemical
</commit_message>
<xml_diff>
--- a/tests/data/excel/test.xlsx
+++ b/tests/data/excel/test.xlsx
@@ -515,7 +515,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L11"/>
+  <dimension ref="A1:L7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -599,17 +599,15 @@
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>chemical1</t>
-        </is>
-      </c>
-      <c r="K2" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+          <t>CONTROL (SEE VEHICLE)</t>
+        </is>
+      </c>
+      <c r="K2" t="n">
+        <v>0</v>
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>TP1</t>
+          <t>TP0</t>
         </is>
       </c>
     </row>
@@ -627,17 +625,15 @@
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>chemical1</t>
-        </is>
-      </c>
-      <c r="K3" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+          <t>CONTROL (SEE VEHICLE)</t>
+        </is>
+      </c>
+      <c r="K3" t="n">
+        <v>0</v>
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>TP1</t>
+          <t>TP0</t>
         </is>
       </c>
     </row>
@@ -655,17 +651,15 @@
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>chemical1</t>
-        </is>
-      </c>
-      <c r="K4" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+          <t>CONTROL (SEE VEHICLE)</t>
+        </is>
+      </c>
+      <c r="K4" t="n">
+        <v>0</v>
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t>TP1</t>
+          <t>TP0</t>
         </is>
       </c>
     </row>
@@ -683,17 +677,15 @@
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>chemical1</t>
-        </is>
-      </c>
-      <c r="K5" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+          <t>CONTROL (SEE VEHICLE)</t>
+        </is>
+      </c>
+      <c r="K5" t="n">
+        <v>0</v>
       </c>
       <c r="L5" t="inlineStr">
         <is>
-          <t>TP1</t>
+          <t>TP0</t>
         </is>
       </c>
     </row>
@@ -707,19 +699,21 @@
       <c r="G6" t="inlineStr"/>
       <c r="H6" t="inlineStr"/>
       <c r="I6" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>CONTROL (SEE VEHICLE)</t>
-        </is>
-      </c>
-      <c r="K6" t="n">
-        <v>0</v>
+          <t>EXTRACTION BLANK</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
       </c>
       <c r="L6" t="inlineStr">
         <is>
-          <t>TP1</t>
+          <t>TP0</t>
         </is>
       </c>
     </row>
@@ -733,125 +727,19 @@
       <c r="G7" t="inlineStr"/>
       <c r="H7" t="inlineStr"/>
       <c r="I7" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>CONTROL (SEE VEHICLE)</t>
-        </is>
-      </c>
-      <c r="K7" t="n">
-        <v>0</v>
+          <t>EXTRACTION BLANK</t>
+        </is>
+      </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
       </c>
       <c r="L7" t="inlineStr">
-        <is>
-          <t>TP1</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr"/>
-      <c r="B8" t="inlineStr"/>
-      <c r="C8" t="inlineStr"/>
-      <c r="D8" t="inlineStr"/>
-      <c r="E8" t="inlineStr"/>
-      <c r="F8" t="inlineStr"/>
-      <c r="G8" t="inlineStr"/>
-      <c r="H8" t="inlineStr"/>
-      <c r="I8" t="n">
-        <v>3</v>
-      </c>
-      <c r="J8" t="inlineStr">
-        <is>
-          <t>CONTROL (SEE VEHICLE)</t>
-        </is>
-      </c>
-      <c r="K8" t="n">
-        <v>0</v>
-      </c>
-      <c r="L8" t="inlineStr">
-        <is>
-          <t>TP1</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr"/>
-      <c r="B9" t="inlineStr"/>
-      <c r="C9" t="inlineStr"/>
-      <c r="D9" t="inlineStr"/>
-      <c r="E9" t="inlineStr"/>
-      <c r="F9" t="inlineStr"/>
-      <c r="G9" t="inlineStr"/>
-      <c r="H9" t="inlineStr"/>
-      <c r="I9" t="n">
-        <v>4</v>
-      </c>
-      <c r="J9" t="inlineStr">
-        <is>
-          <t>CONTROL (SEE VEHICLE)</t>
-        </is>
-      </c>
-      <c r="K9" t="n">
-        <v>0</v>
-      </c>
-      <c r="L9" t="inlineStr">
-        <is>
-          <t>TP1</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr"/>
-      <c r="B10" t="inlineStr"/>
-      <c r="C10" t="inlineStr"/>
-      <c r="D10" t="inlineStr"/>
-      <c r="E10" t="inlineStr"/>
-      <c r="F10" t="inlineStr"/>
-      <c r="G10" t="inlineStr"/>
-      <c r="H10" t="inlineStr"/>
-      <c r="I10" t="n">
-        <v>0</v>
-      </c>
-      <c r="J10" t="inlineStr">
-        <is>
-          <t>EXTRACTION BLANK</t>
-        </is>
-      </c>
-      <c r="K10" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="L10" t="inlineStr">
-        <is>
-          <t>TP0</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr"/>
-      <c r="B11" t="inlineStr"/>
-      <c r="C11" t="inlineStr"/>
-      <c r="D11" t="inlineStr"/>
-      <c r="E11" t="inlineStr"/>
-      <c r="F11" t="inlineStr"/>
-      <c r="G11" t="inlineStr"/>
-      <c r="H11" t="inlineStr"/>
-      <c r="I11" t="n">
-        <v>0</v>
-      </c>
-      <c r="J11" t="inlineStr">
-        <is>
-          <t>EXTRACTION BLANK</t>
-        </is>
-      </c>
-      <c r="K11" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="L11" t="inlineStr">
         <is>
           <t>TP0</t>
         </is>

</xml_diff>

<commit_message>
added timepoints to harvester
</commit_message>
<xml_diff>
--- a/tests/data/excel/test.xlsx
+++ b/tests/data/excel/test.xlsx
@@ -515,7 +515,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L7"/>
+  <dimension ref="A1:L27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -599,15 +599,17 @@
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>CONTROL (SEE VEHICLE)</t>
-        </is>
-      </c>
-      <c r="K2" t="n">
-        <v>0</v>
+          <t>chemical1</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>BMD10</t>
+        </is>
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>TP0</t>
+          <t>TP1</t>
         </is>
       </c>
     </row>
@@ -625,15 +627,17 @@
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>CONTROL (SEE VEHICLE)</t>
-        </is>
-      </c>
-      <c r="K3" t="n">
-        <v>0</v>
+          <t>chemical1</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>BMD10</t>
+        </is>
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>TP0</t>
+          <t>TP1</t>
         </is>
       </c>
     </row>
@@ -651,15 +655,17 @@
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>CONTROL (SEE VEHICLE)</t>
-        </is>
-      </c>
-      <c r="K4" t="n">
-        <v>0</v>
+          <t>chemical1</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>BMD10</t>
+        </is>
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t>TP0</t>
+          <t>TP1</t>
         </is>
       </c>
     </row>
@@ -677,15 +683,17 @@
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>CONTROL (SEE VEHICLE)</t>
-        </is>
-      </c>
-      <c r="K5" t="n">
-        <v>0</v>
+          <t>chemical1</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>BMD10</t>
+        </is>
       </c>
       <c r="L5" t="inlineStr">
         <is>
-          <t>TP0</t>
+          <t>TP1</t>
         </is>
       </c>
     </row>
@@ -699,21 +707,19 @@
       <c r="G6" t="inlineStr"/>
       <c r="H6" t="inlineStr"/>
       <c r="I6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>EXTRACTION BLANK</t>
-        </is>
-      </c>
-      <c r="K6" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+          <t>CONTROL (SEE VEHICLE)</t>
+        </is>
+      </c>
+      <c r="K6" t="n">
+        <v>0</v>
       </c>
       <c r="L6" t="inlineStr">
         <is>
-          <t>TP0</t>
+          <t>TP1</t>
         </is>
       </c>
     </row>
@@ -727,19 +733,557 @@
       <c r="G7" t="inlineStr"/>
       <c r="H7" t="inlineStr"/>
       <c r="I7" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J7" t="inlineStr">
         <is>
+          <t>CONTROL (SEE VEHICLE)</t>
+        </is>
+      </c>
+      <c r="K7" t="n">
+        <v>0</v>
+      </c>
+      <c r="L7" t="inlineStr">
+        <is>
+          <t>TP1</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr"/>
+      <c r="B8" t="inlineStr"/>
+      <c r="C8" t="inlineStr"/>
+      <c r="D8" t="inlineStr"/>
+      <c r="E8" t="inlineStr"/>
+      <c r="F8" t="inlineStr"/>
+      <c r="G8" t="inlineStr"/>
+      <c r="H8" t="inlineStr"/>
+      <c r="I8" t="n">
+        <v>3</v>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>CONTROL (SEE VEHICLE)</t>
+        </is>
+      </c>
+      <c r="K8" t="n">
+        <v>0</v>
+      </c>
+      <c r="L8" t="inlineStr">
+        <is>
+          <t>TP1</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr"/>
+      <c r="B9" t="inlineStr"/>
+      <c r="C9" t="inlineStr"/>
+      <c r="D9" t="inlineStr"/>
+      <c r="E9" t="inlineStr"/>
+      <c r="F9" t="inlineStr"/>
+      <c r="G9" t="inlineStr"/>
+      <c r="H9" t="inlineStr"/>
+      <c r="I9" t="n">
+        <v>4</v>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>CONTROL (SEE VEHICLE)</t>
+        </is>
+      </c>
+      <c r="K9" t="n">
+        <v>0</v>
+      </c>
+      <c r="L9" t="inlineStr">
+        <is>
+          <t>TP1</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr"/>
+      <c r="B10" t="inlineStr"/>
+      <c r="C10" t="inlineStr"/>
+      <c r="D10" t="inlineStr"/>
+      <c r="E10" t="inlineStr"/>
+      <c r="F10" t="inlineStr"/>
+      <c r="G10" t="inlineStr"/>
+      <c r="H10" t="inlineStr"/>
+      <c r="I10" t="n">
+        <v>1</v>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>chemical1</t>
+        </is>
+      </c>
+      <c r="K10" t="inlineStr">
+        <is>
+          <t>BMD10</t>
+        </is>
+      </c>
+      <c r="L10" t="inlineStr">
+        <is>
+          <t>TP2</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr"/>
+      <c r="B11" t="inlineStr"/>
+      <c r="C11" t="inlineStr"/>
+      <c r="D11" t="inlineStr"/>
+      <c r="E11" t="inlineStr"/>
+      <c r="F11" t="inlineStr"/>
+      <c r="G11" t="inlineStr"/>
+      <c r="H11" t="inlineStr"/>
+      <c r="I11" t="n">
+        <v>2</v>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>chemical1</t>
+        </is>
+      </c>
+      <c r="K11" t="inlineStr">
+        <is>
+          <t>BMD10</t>
+        </is>
+      </c>
+      <c r="L11" t="inlineStr">
+        <is>
+          <t>TP2</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr"/>
+      <c r="B12" t="inlineStr"/>
+      <c r="C12" t="inlineStr"/>
+      <c r="D12" t="inlineStr"/>
+      <c r="E12" t="inlineStr"/>
+      <c r="F12" t="inlineStr"/>
+      <c r="G12" t="inlineStr"/>
+      <c r="H12" t="inlineStr"/>
+      <c r="I12" t="n">
+        <v>3</v>
+      </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>chemical1</t>
+        </is>
+      </c>
+      <c r="K12" t="inlineStr">
+        <is>
+          <t>BMD10</t>
+        </is>
+      </c>
+      <c r="L12" t="inlineStr">
+        <is>
+          <t>TP2</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr"/>
+      <c r="B13" t="inlineStr"/>
+      <c r="C13" t="inlineStr"/>
+      <c r="D13" t="inlineStr"/>
+      <c r="E13" t="inlineStr"/>
+      <c r="F13" t="inlineStr"/>
+      <c r="G13" t="inlineStr"/>
+      <c r="H13" t="inlineStr"/>
+      <c r="I13" t="n">
+        <v>4</v>
+      </c>
+      <c r="J13" t="inlineStr">
+        <is>
+          <t>chemical1</t>
+        </is>
+      </c>
+      <c r="K13" t="inlineStr">
+        <is>
+          <t>BMD10</t>
+        </is>
+      </c>
+      <c r="L13" t="inlineStr">
+        <is>
+          <t>TP2</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr"/>
+      <c r="B14" t="inlineStr"/>
+      <c r="C14" t="inlineStr"/>
+      <c r="D14" t="inlineStr"/>
+      <c r="E14" t="inlineStr"/>
+      <c r="F14" t="inlineStr"/>
+      <c r="G14" t="inlineStr"/>
+      <c r="H14" t="inlineStr"/>
+      <c r="I14" t="n">
+        <v>1</v>
+      </c>
+      <c r="J14" t="inlineStr">
+        <is>
+          <t>CONTROL (SEE VEHICLE)</t>
+        </is>
+      </c>
+      <c r="K14" t="n">
+        <v>0</v>
+      </c>
+      <c r="L14" t="inlineStr">
+        <is>
+          <t>TP2</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr"/>
+      <c r="B15" t="inlineStr"/>
+      <c r="C15" t="inlineStr"/>
+      <c r="D15" t="inlineStr"/>
+      <c r="E15" t="inlineStr"/>
+      <c r="F15" t="inlineStr"/>
+      <c r="G15" t="inlineStr"/>
+      <c r="H15" t="inlineStr"/>
+      <c r="I15" t="n">
+        <v>2</v>
+      </c>
+      <c r="J15" t="inlineStr">
+        <is>
+          <t>CONTROL (SEE VEHICLE)</t>
+        </is>
+      </c>
+      <c r="K15" t="n">
+        <v>0</v>
+      </c>
+      <c r="L15" t="inlineStr">
+        <is>
+          <t>TP2</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr"/>
+      <c r="B16" t="inlineStr"/>
+      <c r="C16" t="inlineStr"/>
+      <c r="D16" t="inlineStr"/>
+      <c r="E16" t="inlineStr"/>
+      <c r="F16" t="inlineStr"/>
+      <c r="G16" t="inlineStr"/>
+      <c r="H16" t="inlineStr"/>
+      <c r="I16" t="n">
+        <v>3</v>
+      </c>
+      <c r="J16" t="inlineStr">
+        <is>
+          <t>CONTROL (SEE VEHICLE)</t>
+        </is>
+      </c>
+      <c r="K16" t="n">
+        <v>0</v>
+      </c>
+      <c r="L16" t="inlineStr">
+        <is>
+          <t>TP2</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr"/>
+      <c r="B17" t="inlineStr"/>
+      <c r="C17" t="inlineStr"/>
+      <c r="D17" t="inlineStr"/>
+      <c r="E17" t="inlineStr"/>
+      <c r="F17" t="inlineStr"/>
+      <c r="G17" t="inlineStr"/>
+      <c r="H17" t="inlineStr"/>
+      <c r="I17" t="n">
+        <v>4</v>
+      </c>
+      <c r="J17" t="inlineStr">
+        <is>
+          <t>CONTROL (SEE VEHICLE)</t>
+        </is>
+      </c>
+      <c r="K17" t="n">
+        <v>0</v>
+      </c>
+      <c r="L17" t="inlineStr">
+        <is>
+          <t>TP2</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr"/>
+      <c r="B18" t="inlineStr"/>
+      <c r="C18" t="inlineStr"/>
+      <c r="D18" t="inlineStr"/>
+      <c r="E18" t="inlineStr"/>
+      <c r="F18" t="inlineStr"/>
+      <c r="G18" t="inlineStr"/>
+      <c r="H18" t="inlineStr"/>
+      <c r="I18" t="n">
+        <v>1</v>
+      </c>
+      <c r="J18" t="inlineStr">
+        <is>
+          <t>chemical1</t>
+        </is>
+      </c>
+      <c r="K18" t="inlineStr">
+        <is>
+          <t>BMD10</t>
+        </is>
+      </c>
+      <c r="L18" t="inlineStr">
+        <is>
+          <t>TP3</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr"/>
+      <c r="B19" t="inlineStr"/>
+      <c r="C19" t="inlineStr"/>
+      <c r="D19" t="inlineStr"/>
+      <c r="E19" t="inlineStr"/>
+      <c r="F19" t="inlineStr"/>
+      <c r="G19" t="inlineStr"/>
+      <c r="H19" t="inlineStr"/>
+      <c r="I19" t="n">
+        <v>2</v>
+      </c>
+      <c r="J19" t="inlineStr">
+        <is>
+          <t>chemical1</t>
+        </is>
+      </c>
+      <c r="K19" t="inlineStr">
+        <is>
+          <t>BMD10</t>
+        </is>
+      </c>
+      <c r="L19" t="inlineStr">
+        <is>
+          <t>TP3</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr"/>
+      <c r="B20" t="inlineStr"/>
+      <c r="C20" t="inlineStr"/>
+      <c r="D20" t="inlineStr"/>
+      <c r="E20" t="inlineStr"/>
+      <c r="F20" t="inlineStr"/>
+      <c r="G20" t="inlineStr"/>
+      <c r="H20" t="inlineStr"/>
+      <c r="I20" t="n">
+        <v>3</v>
+      </c>
+      <c r="J20" t="inlineStr">
+        <is>
+          <t>chemical1</t>
+        </is>
+      </c>
+      <c r="K20" t="inlineStr">
+        <is>
+          <t>BMD10</t>
+        </is>
+      </c>
+      <c r="L20" t="inlineStr">
+        <is>
+          <t>TP3</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr"/>
+      <c r="B21" t="inlineStr"/>
+      <c r="C21" t="inlineStr"/>
+      <c r="D21" t="inlineStr"/>
+      <c r="E21" t="inlineStr"/>
+      <c r="F21" t="inlineStr"/>
+      <c r="G21" t="inlineStr"/>
+      <c r="H21" t="inlineStr"/>
+      <c r="I21" t="n">
+        <v>4</v>
+      </c>
+      <c r="J21" t="inlineStr">
+        <is>
+          <t>chemical1</t>
+        </is>
+      </c>
+      <c r="K21" t="inlineStr">
+        <is>
+          <t>BMD10</t>
+        </is>
+      </c>
+      <c r="L21" t="inlineStr">
+        <is>
+          <t>TP3</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr"/>
+      <c r="B22" t="inlineStr"/>
+      <c r="C22" t="inlineStr"/>
+      <c r="D22" t="inlineStr"/>
+      <c r="E22" t="inlineStr"/>
+      <c r="F22" t="inlineStr"/>
+      <c r="G22" t="inlineStr"/>
+      <c r="H22" t="inlineStr"/>
+      <c r="I22" t="n">
+        <v>1</v>
+      </c>
+      <c r="J22" t="inlineStr">
+        <is>
+          <t>CONTROL (SEE VEHICLE)</t>
+        </is>
+      </c>
+      <c r="K22" t="n">
+        <v>0</v>
+      </c>
+      <c r="L22" t="inlineStr">
+        <is>
+          <t>TP3</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr"/>
+      <c r="B23" t="inlineStr"/>
+      <c r="C23" t="inlineStr"/>
+      <c r="D23" t="inlineStr"/>
+      <c r="E23" t="inlineStr"/>
+      <c r="F23" t="inlineStr"/>
+      <c r="G23" t="inlineStr"/>
+      <c r="H23" t="inlineStr"/>
+      <c r="I23" t="n">
+        <v>2</v>
+      </c>
+      <c r="J23" t="inlineStr">
+        <is>
+          <t>CONTROL (SEE VEHICLE)</t>
+        </is>
+      </c>
+      <c r="K23" t="n">
+        <v>0</v>
+      </c>
+      <c r="L23" t="inlineStr">
+        <is>
+          <t>TP3</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr"/>
+      <c r="B24" t="inlineStr"/>
+      <c r="C24" t="inlineStr"/>
+      <c r="D24" t="inlineStr"/>
+      <c r="E24" t="inlineStr"/>
+      <c r="F24" t="inlineStr"/>
+      <c r="G24" t="inlineStr"/>
+      <c r="H24" t="inlineStr"/>
+      <c r="I24" t="n">
+        <v>3</v>
+      </c>
+      <c r="J24" t="inlineStr">
+        <is>
+          <t>CONTROL (SEE VEHICLE)</t>
+        </is>
+      </c>
+      <c r="K24" t="n">
+        <v>0</v>
+      </c>
+      <c r="L24" t="inlineStr">
+        <is>
+          <t>TP3</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr"/>
+      <c r="B25" t="inlineStr"/>
+      <c r="C25" t="inlineStr"/>
+      <c r="D25" t="inlineStr"/>
+      <c r="E25" t="inlineStr"/>
+      <c r="F25" t="inlineStr"/>
+      <c r="G25" t="inlineStr"/>
+      <c r="H25" t="inlineStr"/>
+      <c r="I25" t="n">
+        <v>4</v>
+      </c>
+      <c r="J25" t="inlineStr">
+        <is>
+          <t>CONTROL (SEE VEHICLE)</t>
+        </is>
+      </c>
+      <c r="K25" t="n">
+        <v>0</v>
+      </c>
+      <c r="L25" t="inlineStr">
+        <is>
+          <t>TP3</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr"/>
+      <c r="B26" t="inlineStr"/>
+      <c r="C26" t="inlineStr"/>
+      <c r="D26" t="inlineStr"/>
+      <c r="E26" t="inlineStr"/>
+      <c r="F26" t="inlineStr"/>
+      <c r="G26" t="inlineStr"/>
+      <c r="H26" t="inlineStr"/>
+      <c r="I26" t="n">
+        <v>0</v>
+      </c>
+      <c r="J26" t="inlineStr">
+        <is>
           <t>EXTRACTION BLANK</t>
         </is>
       </c>
-      <c r="K7" t="inlineStr">
+      <c r="K26" t="inlineStr">
         <is>
           <t>0</t>
         </is>
       </c>
-      <c r="L7" t="inlineStr">
+      <c r="L26" t="inlineStr">
+        <is>
+          <t>TP0</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr"/>
+      <c r="B27" t="inlineStr"/>
+      <c r="C27" t="inlineStr"/>
+      <c r="D27" t="inlineStr"/>
+      <c r="E27" t="inlineStr"/>
+      <c r="F27" t="inlineStr"/>
+      <c r="G27" t="inlineStr"/>
+      <c r="H27" t="inlineStr"/>
+      <c r="I27" t="n">
+        <v>0</v>
+      </c>
+      <c r="J27" t="inlineStr">
+        <is>
+          <t>EXTRACTION BLANK</t>
+        </is>
+      </c>
+      <c r="K27" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="L27" t="inlineStr">
         <is>
           <t>TP0</t>
         </is>

</xml_diff>

<commit_message>
added vehicle and tests
</commit_message>
<xml_diff>
--- a/tests/data/excel/test.xlsx
+++ b/tests/data/excel/test.xlsx
@@ -515,7 +515,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L27"/>
+  <dimension ref="A1:M27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -582,6 +582,11 @@
       <c r="L1" s="1" t="inlineStr">
         <is>
           <t>time point</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>vehicle</t>
         </is>
       </c>
     </row>
@@ -612,6 +617,11 @@
           <t>TP1</t>
         </is>
       </c>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>water</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr"/>
@@ -640,6 +650,11 @@
           <t>TP1</t>
         </is>
       </c>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>water</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr"/>
@@ -668,6 +683,11 @@
           <t>TP1</t>
         </is>
       </c>
+      <c r="M4" t="inlineStr">
+        <is>
+          <t>water</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr"/>
@@ -696,6 +716,11 @@
           <t>TP1</t>
         </is>
       </c>
+      <c r="M5" t="inlineStr">
+        <is>
+          <t>water</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr"/>
@@ -711,7 +736,7 @@
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>CONTROL (SEE VEHICLE)</t>
+          <t>CONTROL (water)</t>
         </is>
       </c>
       <c r="K6" t="n">
@@ -720,6 +745,11 @@
       <c r="L6" t="inlineStr">
         <is>
           <t>TP1</t>
+        </is>
+      </c>
+      <c r="M6" t="inlineStr">
+        <is>
+          <t>water</t>
         </is>
       </c>
     </row>
@@ -737,7 +767,7 @@
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>CONTROL (SEE VEHICLE)</t>
+          <t>CONTROL (water)</t>
         </is>
       </c>
       <c r="K7" t="n">
@@ -746,6 +776,11 @@
       <c r="L7" t="inlineStr">
         <is>
           <t>TP1</t>
+        </is>
+      </c>
+      <c r="M7" t="inlineStr">
+        <is>
+          <t>water</t>
         </is>
       </c>
     </row>
@@ -763,7 +798,7 @@
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>CONTROL (SEE VEHICLE)</t>
+          <t>CONTROL (water)</t>
         </is>
       </c>
       <c r="K8" t="n">
@@ -772,6 +807,11 @@
       <c r="L8" t="inlineStr">
         <is>
           <t>TP1</t>
+        </is>
+      </c>
+      <c r="M8" t="inlineStr">
+        <is>
+          <t>water</t>
         </is>
       </c>
     </row>
@@ -789,7 +829,7 @@
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>CONTROL (SEE VEHICLE)</t>
+          <t>CONTROL (water)</t>
         </is>
       </c>
       <c r="K9" t="n">
@@ -798,6 +838,11 @@
       <c r="L9" t="inlineStr">
         <is>
           <t>TP1</t>
+        </is>
+      </c>
+      <c r="M9" t="inlineStr">
+        <is>
+          <t>water</t>
         </is>
       </c>
     </row>
@@ -828,6 +873,11 @@
           <t>TP2</t>
         </is>
       </c>
+      <c r="M10" t="inlineStr">
+        <is>
+          <t>water</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr"/>
@@ -856,6 +906,11 @@
           <t>TP2</t>
         </is>
       </c>
+      <c r="M11" t="inlineStr">
+        <is>
+          <t>water</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr"/>
@@ -884,6 +939,11 @@
           <t>TP2</t>
         </is>
       </c>
+      <c r="M12" t="inlineStr">
+        <is>
+          <t>water</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr"/>
@@ -912,6 +972,11 @@
           <t>TP2</t>
         </is>
       </c>
+      <c r="M13" t="inlineStr">
+        <is>
+          <t>water</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr"/>
@@ -927,7 +992,7 @@
       </c>
       <c r="J14" t="inlineStr">
         <is>
-          <t>CONTROL (SEE VEHICLE)</t>
+          <t>CONTROL (water)</t>
         </is>
       </c>
       <c r="K14" t="n">
@@ -936,6 +1001,11 @@
       <c r="L14" t="inlineStr">
         <is>
           <t>TP2</t>
+        </is>
+      </c>
+      <c r="M14" t="inlineStr">
+        <is>
+          <t>water</t>
         </is>
       </c>
     </row>
@@ -953,7 +1023,7 @@
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>CONTROL (SEE VEHICLE)</t>
+          <t>CONTROL (water)</t>
         </is>
       </c>
       <c r="K15" t="n">
@@ -962,6 +1032,11 @@
       <c r="L15" t="inlineStr">
         <is>
           <t>TP2</t>
+        </is>
+      </c>
+      <c r="M15" t="inlineStr">
+        <is>
+          <t>water</t>
         </is>
       </c>
     </row>
@@ -979,7 +1054,7 @@
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>CONTROL (SEE VEHICLE)</t>
+          <t>CONTROL (water)</t>
         </is>
       </c>
       <c r="K16" t="n">
@@ -988,6 +1063,11 @@
       <c r="L16" t="inlineStr">
         <is>
           <t>TP2</t>
+        </is>
+      </c>
+      <c r="M16" t="inlineStr">
+        <is>
+          <t>water</t>
         </is>
       </c>
     </row>
@@ -1005,7 +1085,7 @@
       </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>CONTROL (SEE VEHICLE)</t>
+          <t>CONTROL (water)</t>
         </is>
       </c>
       <c r="K17" t="n">
@@ -1014,6 +1094,11 @@
       <c r="L17" t="inlineStr">
         <is>
           <t>TP2</t>
+        </is>
+      </c>
+      <c r="M17" t="inlineStr">
+        <is>
+          <t>water</t>
         </is>
       </c>
     </row>
@@ -1044,6 +1129,11 @@
           <t>TP3</t>
         </is>
       </c>
+      <c r="M18" t="inlineStr">
+        <is>
+          <t>water</t>
+        </is>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr"/>
@@ -1072,6 +1162,11 @@
           <t>TP3</t>
         </is>
       </c>
+      <c r="M19" t="inlineStr">
+        <is>
+          <t>water</t>
+        </is>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr"/>
@@ -1100,6 +1195,11 @@
           <t>TP3</t>
         </is>
       </c>
+      <c r="M20" t="inlineStr">
+        <is>
+          <t>water</t>
+        </is>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr"/>
@@ -1128,6 +1228,11 @@
           <t>TP3</t>
         </is>
       </c>
+      <c r="M21" t="inlineStr">
+        <is>
+          <t>water</t>
+        </is>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr"/>
@@ -1143,7 +1248,7 @@
       </c>
       <c r="J22" t="inlineStr">
         <is>
-          <t>CONTROL (SEE VEHICLE)</t>
+          <t>CONTROL (water)</t>
         </is>
       </c>
       <c r="K22" t="n">
@@ -1152,6 +1257,11 @@
       <c r="L22" t="inlineStr">
         <is>
           <t>TP3</t>
+        </is>
+      </c>
+      <c r="M22" t="inlineStr">
+        <is>
+          <t>water</t>
         </is>
       </c>
     </row>
@@ -1169,7 +1279,7 @@
       </c>
       <c r="J23" t="inlineStr">
         <is>
-          <t>CONTROL (SEE VEHICLE)</t>
+          <t>CONTROL (water)</t>
         </is>
       </c>
       <c r="K23" t="n">
@@ -1178,6 +1288,11 @@
       <c r="L23" t="inlineStr">
         <is>
           <t>TP3</t>
+        </is>
+      </c>
+      <c r="M23" t="inlineStr">
+        <is>
+          <t>water</t>
         </is>
       </c>
     </row>
@@ -1195,7 +1310,7 @@
       </c>
       <c r="J24" t="inlineStr">
         <is>
-          <t>CONTROL (SEE VEHICLE)</t>
+          <t>CONTROL (water)</t>
         </is>
       </c>
       <c r="K24" t="n">
@@ -1204,6 +1319,11 @@
       <c r="L24" t="inlineStr">
         <is>
           <t>TP3</t>
+        </is>
+      </c>
+      <c r="M24" t="inlineStr">
+        <is>
+          <t>water</t>
         </is>
       </c>
     </row>
@@ -1221,7 +1341,7 @@
       </c>
       <c r="J25" t="inlineStr">
         <is>
-          <t>CONTROL (SEE VEHICLE)</t>
+          <t>CONTROL (water)</t>
         </is>
       </c>
       <c r="K25" t="n">
@@ -1230,6 +1350,11 @@
       <c r="L25" t="inlineStr">
         <is>
           <t>TP3</t>
+        </is>
+      </c>
+      <c r="M25" t="inlineStr">
+        <is>
+          <t>water</t>
         </is>
       </c>
     </row>
@@ -1260,6 +1385,7 @@
           <t>TP0</t>
         </is>
       </c>
+      <c r="M26" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr"/>
@@ -1288,6 +1414,7 @@
           <t>TP0</t>
         </is>
       </c>
+      <c r="M27" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Added hash_id to spreadsheet
</commit_message>
<xml_diff>
--- a/tests/data/excel/test.xlsx
+++ b/tests/data/excel/test.xlsx
@@ -515,7 +515,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M27"/>
+  <dimension ref="A1:N27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -587,6 +587,11 @@
       <c r="M1" s="1" t="inlineStr">
         <is>
           <t>vehicle</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>PrecisionTox short identifier</t>
         </is>
       </c>
     </row>
@@ -622,6 +627,11 @@
           <t>water</t>
         </is>
       </c>
+      <c r="N2" t="inlineStr">
+        <is>
+          <t>XAA---LA1</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr"/>
@@ -655,6 +665,11 @@
           <t>water</t>
         </is>
       </c>
+      <c r="N3" t="inlineStr">
+        <is>
+          <t>XAA---LA2</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr"/>
@@ -688,6 +703,11 @@
           <t>water</t>
         </is>
       </c>
+      <c r="N4" t="inlineStr">
+        <is>
+          <t>XAA---LA3</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr"/>
@@ -721,6 +741,11 @@
           <t>water</t>
         </is>
       </c>
+      <c r="N5" t="inlineStr">
+        <is>
+          <t>XAA---LA4</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr"/>
@@ -752,6 +777,11 @@
           <t>water</t>
         </is>
       </c>
+      <c r="N6" t="inlineStr">
+        <is>
+          <t>XAA---LA1</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr"/>
@@ -783,6 +813,11 @@
           <t>water</t>
         </is>
       </c>
+      <c r="N7" t="inlineStr">
+        <is>
+          <t>XAA---LA2</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr"/>
@@ -814,6 +849,11 @@
           <t>water</t>
         </is>
       </c>
+      <c r="N8" t="inlineStr">
+        <is>
+          <t>XAA---LA3</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr"/>
@@ -845,6 +885,11 @@
           <t>water</t>
         </is>
       </c>
+      <c r="N9" t="inlineStr">
+        <is>
+          <t>XAA---LA4</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr"/>
@@ -878,6 +923,11 @@
           <t>water</t>
         </is>
       </c>
+      <c r="N10" t="inlineStr">
+        <is>
+          <t>XAA---LB1</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr"/>
@@ -911,6 +961,11 @@
           <t>water</t>
         </is>
       </c>
+      <c r="N11" t="inlineStr">
+        <is>
+          <t>XAA---LB2</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr"/>
@@ -944,6 +999,11 @@
           <t>water</t>
         </is>
       </c>
+      <c r="N12" t="inlineStr">
+        <is>
+          <t>XAA---LB3</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr"/>
@@ -977,6 +1037,11 @@
           <t>water</t>
         </is>
       </c>
+      <c r="N13" t="inlineStr">
+        <is>
+          <t>XAA---LB4</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr"/>
@@ -1008,6 +1073,11 @@
           <t>water</t>
         </is>
       </c>
+      <c r="N14" t="inlineStr">
+        <is>
+          <t>XAA---LB1</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr"/>
@@ -1039,6 +1109,11 @@
           <t>water</t>
         </is>
       </c>
+      <c r="N15" t="inlineStr">
+        <is>
+          <t>XAA---LB2</t>
+        </is>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr"/>
@@ -1070,6 +1145,11 @@
           <t>water</t>
         </is>
       </c>
+      <c r="N16" t="inlineStr">
+        <is>
+          <t>XAA---LB3</t>
+        </is>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr"/>
@@ -1101,6 +1181,11 @@
           <t>water</t>
         </is>
       </c>
+      <c r="N17" t="inlineStr">
+        <is>
+          <t>XAA---LB4</t>
+        </is>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr"/>
@@ -1134,6 +1219,11 @@
           <t>water</t>
         </is>
       </c>
+      <c r="N18" t="inlineStr">
+        <is>
+          <t>XAA---LC1</t>
+        </is>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr"/>
@@ -1167,6 +1257,11 @@
           <t>water</t>
         </is>
       </c>
+      <c r="N19" t="inlineStr">
+        <is>
+          <t>XAA---LC2</t>
+        </is>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr"/>
@@ -1200,6 +1295,11 @@
           <t>water</t>
         </is>
       </c>
+      <c r="N20" t="inlineStr">
+        <is>
+          <t>XAA---LC3</t>
+        </is>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr"/>
@@ -1233,6 +1333,11 @@
           <t>water</t>
         </is>
       </c>
+      <c r="N21" t="inlineStr">
+        <is>
+          <t>XAA---LC4</t>
+        </is>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr"/>
@@ -1264,6 +1369,11 @@
           <t>water</t>
         </is>
       </c>
+      <c r="N22" t="inlineStr">
+        <is>
+          <t>XAA---LC1</t>
+        </is>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr"/>
@@ -1295,6 +1405,11 @@
           <t>water</t>
         </is>
       </c>
+      <c r="N23" t="inlineStr">
+        <is>
+          <t>XAA---LC2</t>
+        </is>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr"/>
@@ -1326,6 +1441,11 @@
           <t>water</t>
         </is>
       </c>
+      <c r="N24" t="inlineStr">
+        <is>
+          <t>XAA---LC3</t>
+        </is>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr"/>
@@ -1357,6 +1477,11 @@
           <t>water</t>
         </is>
       </c>
+      <c r="N25" t="inlineStr">
+        <is>
+          <t>XAA---LC4</t>
+        </is>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr"/>
@@ -1368,7 +1493,7 @@
       <c r="G26" t="inlineStr"/>
       <c r="H26" t="inlineStr"/>
       <c r="I26" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J26" t="inlineStr">
         <is>
@@ -1386,6 +1511,11 @@
         </is>
       </c>
       <c r="M26" t="inlineStr"/>
+      <c r="N26" t="inlineStr">
+        <is>
+          <t>XAA998ZS1</t>
+        </is>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr"/>
@@ -1397,7 +1527,7 @@
       <c r="G27" t="inlineStr"/>
       <c r="H27" t="inlineStr"/>
       <c r="I27" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J27" t="inlineStr">
         <is>
@@ -1415,6 +1545,11 @@
         </is>
       </c>
       <c r="M27" t="inlineStr"/>
+      <c r="N27" t="inlineStr">
+        <is>
+          <t>XAA998ZS2</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
minor refactoring to prevent long functions
</commit_message>
<xml_diff>
--- a/tests/data/excel/test.xlsx
+++ b/tests/data/excel/test.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -472,33 +472,96 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
+      <c r="A2" t="inlineStr"/>
+      <c r="B2" t="inlineStr"/>
+      <c r="C2" t="inlineStr"/>
+      <c r="D2" t="inlineStr"/>
+      <c r="E2" t="inlineStr"/>
+      <c r="F2" t="inlineStr"/>
+      <c r="G2" t="inlineStr"/>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr"/>
+      <c r="B3" t="inlineStr"/>
+      <c r="C3" t="inlineStr"/>
+      <c r="D3" t="inlineStr"/>
+      <c r="E3" t="inlineStr"/>
+      <c r="F3" t="inlineStr"/>
+      <c r="G3" t="inlineStr"/>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr"/>
+      <c r="B4" t="inlineStr"/>
+      <c r="C4" t="inlineStr"/>
+      <c r="D4" t="inlineStr"/>
+      <c r="E4" t="inlineStr"/>
+      <c r="F4" t="inlineStr"/>
+      <c r="G4" t="inlineStr"/>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr"/>
+      <c r="B5" t="inlineStr"/>
+      <c r="C5" t="inlineStr"/>
+      <c r="D5" t="inlineStr"/>
+      <c r="E5" t="inlineStr"/>
+      <c r="F5" t="inlineStr"/>
+      <c r="G5" t="inlineStr"/>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr"/>
+      <c r="B6" t="inlineStr"/>
+      <c r="C6" t="inlineStr"/>
+      <c r="D6" t="inlineStr"/>
+      <c r="E6" t="inlineStr"/>
+      <c r="F6" t="inlineStr"/>
+      <c r="G6" t="inlineStr"/>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr"/>
+      <c r="B7" t="inlineStr"/>
+      <c r="C7" t="inlineStr"/>
+      <c r="D7" t="inlineStr"/>
+      <c r="E7" t="inlineStr"/>
+      <c r="F7" t="inlineStr"/>
+      <c r="G7" t="inlineStr"/>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr"/>
+      <c r="B8" t="inlineStr"/>
+      <c r="C8" t="inlineStr"/>
+      <c r="D8" t="inlineStr"/>
+      <c r="E8" t="inlineStr"/>
+      <c r="F8" t="inlineStr"/>
+      <c r="G8" t="inlineStr"/>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
         <is>
           <t>KIT</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
+      <c r="B9" t="inlineStr">
         <is>
           <t>organism1</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
+      <c r="C9" t="inlineStr">
         <is>
           <t>AA</t>
         </is>
       </c>
-      <c r="D2" t="n">
+      <c r="D9" t="n">
         <v>4</v>
       </c>
-      <c r="E2" t="n">
+      <c r="E9" t="n">
         <v>2</v>
       </c>
-      <c r="F2" t="inlineStr">
+      <c r="F9" t="inlineStr">
         <is>
           <t>2018-01-01</t>
         </is>
       </c>
-      <c r="G2" t="inlineStr">
+      <c r="G9" t="inlineStr">
         <is>
           <t>2019-01-02</t>
         </is>
@@ -757,7 +820,7 @@
       <c r="G6" t="inlineStr"/>
       <c r="H6" t="inlineStr"/>
       <c r="I6" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J6" t="inlineStr">
         <is>
@@ -779,7 +842,7 @@
       </c>
       <c r="N6" t="inlineStr">
         <is>
-          <t>XAA001AZ1</t>
+          <t>XAA001AZ0</t>
         </is>
       </c>
     </row>
@@ -793,7 +856,7 @@
       <c r="G7" t="inlineStr"/>
       <c r="H7" t="inlineStr"/>
       <c r="I7" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J7" t="inlineStr">
         <is>
@@ -815,7 +878,7 @@
       </c>
       <c r="N7" t="inlineStr">
         <is>
-          <t>XAA001AZ2</t>
+          <t>XAA001AZ1</t>
         </is>
       </c>
     </row>
@@ -829,7 +892,7 @@
       <c r="G8" t="inlineStr"/>
       <c r="H8" t="inlineStr"/>
       <c r="I8" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J8" t="inlineStr">
         <is>
@@ -851,7 +914,7 @@
       </c>
       <c r="N8" t="inlineStr">
         <is>
-          <t>XAA001AZ3</t>
+          <t>XAA001AZ2</t>
         </is>
       </c>
     </row>
@@ -865,7 +928,7 @@
       <c r="G9" t="inlineStr"/>
       <c r="H9" t="inlineStr"/>
       <c r="I9" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J9" t="inlineStr">
         <is>
@@ -887,7 +950,7 @@
       </c>
       <c r="N9" t="inlineStr">
         <is>
-          <t>XAA001AZ4</t>
+          <t>XAA001AZ3</t>
         </is>
       </c>
     </row>
@@ -1053,7 +1116,7 @@
       <c r="G14" t="inlineStr"/>
       <c r="H14" t="inlineStr"/>
       <c r="I14" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J14" t="inlineStr">
         <is>
@@ -1075,7 +1138,7 @@
       </c>
       <c r="N14" t="inlineStr">
         <is>
-          <t>XAA001BZ1</t>
+          <t>XAA001BZ0</t>
         </is>
       </c>
     </row>
@@ -1089,7 +1152,7 @@
       <c r="G15" t="inlineStr"/>
       <c r="H15" t="inlineStr"/>
       <c r="I15" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J15" t="inlineStr">
         <is>
@@ -1111,7 +1174,7 @@
       </c>
       <c r="N15" t="inlineStr">
         <is>
-          <t>XAA001BZ2</t>
+          <t>XAA001BZ1</t>
         </is>
       </c>
     </row>
@@ -1125,7 +1188,7 @@
       <c r="G16" t="inlineStr"/>
       <c r="H16" t="inlineStr"/>
       <c r="I16" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J16" t="inlineStr">
         <is>
@@ -1147,7 +1210,7 @@
       </c>
       <c r="N16" t="inlineStr">
         <is>
-          <t>XAA001BZ3</t>
+          <t>XAA001BZ2</t>
         </is>
       </c>
     </row>
@@ -1161,7 +1224,7 @@
       <c r="G17" t="inlineStr"/>
       <c r="H17" t="inlineStr"/>
       <c r="I17" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J17" t="inlineStr">
         <is>
@@ -1183,7 +1246,7 @@
       </c>
       <c r="N17" t="inlineStr">
         <is>
-          <t>XAA001BZ4</t>
+          <t>XAA001BZ3</t>
         </is>
       </c>
     </row>
@@ -1349,7 +1412,7 @@
       <c r="G22" t="inlineStr"/>
       <c r="H22" t="inlineStr"/>
       <c r="I22" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J22" t="inlineStr">
         <is>
@@ -1371,7 +1434,7 @@
       </c>
       <c r="N22" t="inlineStr">
         <is>
-          <t>XAA001CZ1</t>
+          <t>XAA001CZ0</t>
         </is>
       </c>
     </row>
@@ -1385,7 +1448,7 @@
       <c r="G23" t="inlineStr"/>
       <c r="H23" t="inlineStr"/>
       <c r="I23" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J23" t="inlineStr">
         <is>
@@ -1407,7 +1470,7 @@
       </c>
       <c r="N23" t="inlineStr">
         <is>
-          <t>XAA001CZ2</t>
+          <t>XAA001CZ1</t>
         </is>
       </c>
     </row>
@@ -1421,7 +1484,7 @@
       <c r="G24" t="inlineStr"/>
       <c r="H24" t="inlineStr"/>
       <c r="I24" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J24" t="inlineStr">
         <is>
@@ -1443,7 +1506,7 @@
       </c>
       <c r="N24" t="inlineStr">
         <is>
-          <t>XAA001CZ3</t>
+          <t>XAA001CZ2</t>
         </is>
       </c>
     </row>
@@ -1457,7 +1520,7 @@
       <c r="G25" t="inlineStr"/>
       <c r="H25" t="inlineStr"/>
       <c r="I25" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J25" t="inlineStr">
         <is>
@@ -1479,7 +1542,7 @@
       </c>
       <c r="N25" t="inlineStr">
         <is>
-          <t>XAA001CZ4</t>
+          <t>XAA001CZ3</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
splitted excel related functions intead their own client
</commit_message>
<xml_diff>
--- a/tests/data/excel/test.xlsx
+++ b/tests/data/excel/test.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="64">
   <si>
     <t>partner</t>
   </si>
@@ -74,7 +74,7 @@
     <t>Box No.</t>
   </si>
   <si>
-    <t>FreezerBoxID</t>
+    <t>FreezerBox identifier</t>
   </si>
   <si>
     <t>Sample position in box</t>
@@ -213,7 +213,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="5">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -222,33 +222,23 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="15.0"/>
+      <sz val="14"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12.0"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
+      <sz val="16"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
       <family val="2"/>
-      <scheme val="minor"/>
     </font>
     <font>
-      <sz val="13.5"/>
+      <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="4">
@@ -260,13 +250,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF008080"/>
+        <fgColor rgb="FFCCCCCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFEFEFEF"/>
+        <fgColor rgb="FF008080"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -280,32 +270,32 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color rgb="FF000000"/>
+      <left style="thin">
+        <color auto="1"/>
       </left>
-      <right style="medium">
-        <color rgb="FF000000"/>
+      <right style="thin">
+        <color auto="1"/>
       </right>
-      <top style="medium">
-        <color rgb="FF000000"/>
+      <top style="thin">
+        <color auto="1"/>
       </top>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
+      <bottom style="thin">
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
+      <left style="thick">
+        <color auto="1"/>
       </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
+      <right style="thick">
+        <color auto="1"/>
       </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
+      <top style="thick">
+        <color auto="1"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
+      <bottom style="thick">
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -313,17 +303,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -625,70 +614,70 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="10" width="25.7109375" customWidth="1"/>
+    <col min="1" max="10" width="25.7109375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
+    <row r="1" spans="1:10" s="2" customFormat="1" ht="50" customHeight="1">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:10">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="2">
+      <c r="D2" s="1">
         <v>4</v>
       </c>
-      <c r="E2" s="2">
+      <c r="E2" s="1">
         <v>4</v>
       </c>
-      <c r="F2" s="2">
+      <c r="F2" s="1">
         <v>2</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="G2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="H2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="I2" s="2">
+      <c r="I2" s="1">
         <v>3</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="J2" s="1" t="s">
         <v>15</v>
       </c>
     </row>
@@ -705,708 +694,497 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="25.7109375" customWidth="1"/>
-    <col min="2" max="2" width="30.7109375" customWidth="1"/>
-    <col min="3" max="4" width="15.7109375" customWidth="1"/>
-    <col min="4" max="4" width="20.7109375" customWidth="1"/>
-    <col min="5" max="5" width="30.7109375" customWidth="1"/>
-    <col min="6" max="7" width="35.7109375" customWidth="1"/>
-    <col min="8" max="8" width="30.7109375" customWidth="1"/>
-    <col min="9" max="9" width="13.7109375" customWidth="1"/>
-    <col min="10" max="10" width="30.7109375" customWidth="1"/>
-    <col min="11" max="12" width="15.7109375" customWidth="1"/>
-    <col min="13" max="13" width="35.7109375" customWidth="1"/>
-    <col min="14" max="26" width="1.7109375" customWidth="1"/>
+    <col min="1" max="1" width="25.7109375" style="3" customWidth="1"/>
+    <col min="2" max="2" width="30.7109375" style="3" customWidth="1"/>
+    <col min="3" max="4" width="15.7109375" style="3" customWidth="1"/>
+    <col min="4" max="4" width="20.7109375" style="3" customWidth="1"/>
+    <col min="5" max="8" width="30.7109375" style="3" customWidth="1"/>
+    <col min="9" max="9" width="15.7109375" style="1" customWidth="1"/>
+    <col min="10" max="10" width="30.7109375" style="1" customWidth="1"/>
+    <col min="11" max="12" width="15.7109375" style="1" customWidth="1"/>
+    <col min="13" max="13" width="30.7109375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="3" customFormat="1" ht="50" customHeight="1">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:13" s="2" customFormat="1" ht="50" customHeight="1">
+      <c r="A1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L1" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="M1" s="2" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:13">
-      <c r="A2" s="2"/>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-      <c r="I2" s="4">
+      <c r="I2" s="1">
         <v>1</v>
       </c>
-      <c r="J2" s="4" t="s">
+      <c r="J2" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="K2" s="4" t="s">
+      <c r="K2" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="L2" s="4" t="s">
+      <c r="L2" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="M2" s="4" t="s">
+      <c r="M2" s="1" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:13">
-      <c r="A3" s="2"/>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="4">
+      <c r="I3" s="1">
         <v>2</v>
       </c>
-      <c r="J3" s="4" t="s">
+      <c r="J3" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="K3" s="4" t="s">
+      <c r="K3" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="L3" s="4" t="s">
+      <c r="L3" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="M3" s="4" t="s">
+      <c r="M3" s="1" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:13">
-      <c r="A4" s="2"/>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="4">
+      <c r="I4" s="1">
         <v>3</v>
       </c>
-      <c r="J4" s="4" t="s">
+      <c r="J4" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="K4" s="4" t="s">
+      <c r="K4" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="L4" s="4" t="s">
+      <c r="L4" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="M4" s="4" t="s">
+      <c r="M4" s="1" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="5" spans="1:13">
-      <c r="A5" s="2"/>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2"/>
-      <c r="I5" s="4">
+      <c r="I5" s="1">
         <v>4</v>
       </c>
-      <c r="J5" s="4" t="s">
+      <c r="J5" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="K5" s="4" t="s">
+      <c r="K5" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="L5" s="4" t="s">
+      <c r="L5" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="M5" s="4" t="s">
+      <c r="M5" s="1" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="6" spans="1:13">
-      <c r="A6" s="2"/>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
-      <c r="I6" s="4">
+      <c r="I6" s="1">
         <v>1</v>
       </c>
-      <c r="J6" s="4" t="s">
+      <c r="J6" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="K6" s="4">
-        <v>0</v>
-      </c>
-      <c r="L6" s="4" t="s">
+      <c r="K6" s="1">
+        <v>0</v>
+      </c>
+      <c r="L6" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="M6" s="4" t="s">
+      <c r="M6" s="1" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="7" spans="1:13">
-      <c r="A7" s="2"/>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
-      <c r="H7" s="2"/>
-      <c r="I7" s="4">
+      <c r="I7" s="1">
         <v>2</v>
       </c>
-      <c r="J7" s="4" t="s">
+      <c r="J7" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="K7" s="4">
-        <v>0</v>
-      </c>
-      <c r="L7" s="4" t="s">
+      <c r="K7" s="1">
+        <v>0</v>
+      </c>
+      <c r="L7" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="M7" s="4" t="s">
+      <c r="M7" s="1" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="8" spans="1:13">
-      <c r="A8" s="2"/>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2"/>
-      <c r="I8" s="4">
+      <c r="I8" s="1">
         <v>3</v>
       </c>
-      <c r="J8" s="4" t="s">
+      <c r="J8" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="K8" s="4">
-        <v>0</v>
-      </c>
-      <c r="L8" s="4" t="s">
+      <c r="K8" s="1">
+        <v>0</v>
+      </c>
+      <c r="L8" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="M8" s="4" t="s">
+      <c r="M8" s="1" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="9" spans="1:13">
-      <c r="A9" s="2"/>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
-      <c r="H9" s="2"/>
-      <c r="I9" s="4">
+      <c r="I9" s="1">
         <v>4</v>
       </c>
-      <c r="J9" s="4" t="s">
+      <c r="J9" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="K9" s="4">
-        <v>0</v>
-      </c>
-      <c r="L9" s="4" t="s">
+      <c r="K9" s="1">
+        <v>0</v>
+      </c>
+      <c r="L9" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="M9" s="4" t="s">
+      <c r="M9" s="1" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="10" spans="1:13">
-      <c r="A10" s="2"/>
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
-      <c r="H10" s="2"/>
-      <c r="I10" s="4">
+      <c r="I10" s="1">
         <v>1</v>
       </c>
-      <c r="J10" s="4" t="s">
+      <c r="J10" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="K10" s="4" t="s">
+      <c r="K10" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="L10" s="4" t="s">
+      <c r="L10" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="M10" s="4" t="s">
+      <c r="M10" s="1" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="11" spans="1:13">
-      <c r="A11" s="2"/>
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
-      <c r="H11" s="2"/>
-      <c r="I11" s="4">
+      <c r="I11" s="1">
         <v>2</v>
       </c>
-      <c r="J11" s="4" t="s">
+      <c r="J11" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="K11" s="4" t="s">
+      <c r="K11" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="L11" s="4" t="s">
+      <c r="L11" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="M11" s="4" t="s">
+      <c r="M11" s="1" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="12" spans="1:13">
-      <c r="A12" s="2"/>
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
-      <c r="G12" s="2"/>
-      <c r="H12" s="2"/>
-      <c r="I12" s="4">
+      <c r="I12" s="1">
         <v>3</v>
       </c>
-      <c r="J12" s="4" t="s">
+      <c r="J12" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="K12" s="4" t="s">
+      <c r="K12" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="L12" s="4" t="s">
+      <c r="L12" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="M12" s="4" t="s">
+      <c r="M12" s="1" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="13" spans="1:13">
-      <c r="A13" s="2"/>
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
-      <c r="G13" s="2"/>
-      <c r="H13" s="2"/>
-      <c r="I13" s="4">
+      <c r="I13" s="1">
         <v>4</v>
       </c>
-      <c r="J13" s="4" t="s">
+      <c r="J13" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="K13" s="4" t="s">
+      <c r="K13" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="L13" s="4" t="s">
+      <c r="L13" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="M13" s="4" t="s">
+      <c r="M13" s="1" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="14" spans="1:13">
-      <c r="A14" s="2"/>
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
-      <c r="G14" s="2"/>
-      <c r="H14" s="2"/>
-      <c r="I14" s="4">
+      <c r="I14" s="1">
         <v>1</v>
       </c>
-      <c r="J14" s="4" t="s">
+      <c r="J14" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="K14" s="4">
-        <v>0</v>
-      </c>
-      <c r="L14" s="4" t="s">
+      <c r="K14" s="1">
+        <v>0</v>
+      </c>
+      <c r="L14" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="M14" s="4" t="s">
+      <c r="M14" s="1" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="15" spans="1:13">
-      <c r="A15" s="2"/>
-      <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
-      <c r="G15" s="2"/>
-      <c r="H15" s="2"/>
-      <c r="I15" s="4">
+      <c r="I15" s="1">
         <v>2</v>
       </c>
-      <c r="J15" s="4" t="s">
+      <c r="J15" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="K15" s="4">
-        <v>0</v>
-      </c>
-      <c r="L15" s="4" t="s">
+      <c r="K15" s="1">
+        <v>0</v>
+      </c>
+      <c r="L15" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="M15" s="4" t="s">
+      <c r="M15" s="1" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="16" spans="1:13">
-      <c r="A16" s="2"/>
-      <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
-      <c r="G16" s="2"/>
-      <c r="H16" s="2"/>
-      <c r="I16" s="4">
+      <c r="I16" s="1">
         <v>3</v>
       </c>
-      <c r="J16" s="4" t="s">
+      <c r="J16" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="K16" s="4">
-        <v>0</v>
-      </c>
-      <c r="L16" s="4" t="s">
+      <c r="K16" s="1">
+        <v>0</v>
+      </c>
+      <c r="L16" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="M16" s="4" t="s">
+      <c r="M16" s="1" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="17" spans="1:13">
-      <c r="A17" s="2"/>
-      <c r="B17" s="2"/>
-      <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
-      <c r="F17" s="2"/>
-      <c r="G17" s="2"/>
-      <c r="H17" s="2"/>
-      <c r="I17" s="4">
+    <row r="17" spans="9:13">
+      <c r="I17" s="1">
         <v>4</v>
       </c>
-      <c r="J17" s="4" t="s">
+      <c r="J17" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="K17" s="4">
-        <v>0</v>
-      </c>
-      <c r="L17" s="4" t="s">
+      <c r="K17" s="1">
+        <v>0</v>
+      </c>
+      <c r="L17" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="M17" s="4" t="s">
+      <c r="M17" s="1" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="18" spans="1:13">
-      <c r="A18" s="2"/>
-      <c r="B18" s="2"/>
-      <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
-      <c r="F18" s="2"/>
-      <c r="G18" s="2"/>
-      <c r="H18" s="2"/>
-      <c r="I18" s="4">
+    <row r="18" spans="9:13">
+      <c r="I18" s="1">
         <v>1</v>
       </c>
-      <c r="J18" s="4" t="s">
+      <c r="J18" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="K18" s="4" t="s">
+      <c r="K18" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="L18" s="4" t="s">
+      <c r="L18" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="M18" s="4" t="s">
+      <c r="M18" s="1" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="19" spans="1:13">
-      <c r="A19" s="2"/>
-      <c r="B19" s="2"/>
-      <c r="C19" s="2"/>
-      <c r="D19" s="2"/>
-      <c r="E19" s="2"/>
-      <c r="F19" s="2"/>
-      <c r="G19" s="2"/>
-      <c r="H19" s="2"/>
-      <c r="I19" s="4">
+    <row r="19" spans="9:13">
+      <c r="I19" s="1">
         <v>2</v>
       </c>
-      <c r="J19" s="4" t="s">
+      <c r="J19" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="K19" s="4" t="s">
+      <c r="K19" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="L19" s="4" t="s">
+      <c r="L19" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="M19" s="4" t="s">
+      <c r="M19" s="1" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="20" spans="1:13">
-      <c r="A20" s="2"/>
-      <c r="B20" s="2"/>
-      <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
-      <c r="G20" s="2"/>
-      <c r="H20" s="2"/>
-      <c r="I20" s="4">
+    <row r="20" spans="9:13">
+      <c r="I20" s="1">
         <v>3</v>
       </c>
-      <c r="J20" s="4" t="s">
+      <c r="J20" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="K20" s="4" t="s">
+      <c r="K20" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="L20" s="4" t="s">
+      <c r="L20" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="M20" s="4" t="s">
+      <c r="M20" s="1" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="21" spans="1:13">
-      <c r="A21" s="2"/>
-      <c r="B21" s="2"/>
-      <c r="C21" s="2"/>
-      <c r="D21" s="2"/>
-      <c r="E21" s="2"/>
-      <c r="F21" s="2"/>
-      <c r="G21" s="2"/>
-      <c r="H21" s="2"/>
-      <c r="I21" s="4">
+    <row r="21" spans="9:13">
+      <c r="I21" s="1">
         <v>4</v>
       </c>
-      <c r="J21" s="4" t="s">
+      <c r="J21" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="K21" s="4" t="s">
+      <c r="K21" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="L21" s="4" t="s">
+      <c r="L21" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="M21" s="4" t="s">
+      <c r="M21" s="1" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="22" spans="1:13">
-      <c r="A22" s="2"/>
-      <c r="B22" s="2"/>
-      <c r="C22" s="2"/>
-      <c r="D22" s="2"/>
-      <c r="E22" s="2"/>
-      <c r="F22" s="2"/>
-      <c r="G22" s="2"/>
-      <c r="H22" s="2"/>
-      <c r="I22" s="4">
+    <row r="22" spans="9:13">
+      <c r="I22" s="1">
         <v>1</v>
       </c>
-      <c r="J22" s="4" t="s">
+      <c r="J22" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="K22" s="4">
-        <v>0</v>
-      </c>
-      <c r="L22" s="4" t="s">
+      <c r="K22" s="1">
+        <v>0</v>
+      </c>
+      <c r="L22" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="M22" s="4" t="s">
+      <c r="M22" s="1" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="23" spans="1:13">
-      <c r="A23" s="2"/>
-      <c r="B23" s="2"/>
-      <c r="C23" s="2"/>
-      <c r="D23" s="2"/>
-      <c r="E23" s="2"/>
-      <c r="F23" s="2"/>
-      <c r="G23" s="2"/>
-      <c r="H23" s="2"/>
-      <c r="I23" s="4">
+    <row r="23" spans="9:13">
+      <c r="I23" s="1">
         <v>2</v>
       </c>
-      <c r="J23" s="4" t="s">
+      <c r="J23" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="K23" s="4">
-        <v>0</v>
-      </c>
-      <c r="L23" s="4" t="s">
+      <c r="K23" s="1">
+        <v>0</v>
+      </c>
+      <c r="L23" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="M23" s="4" t="s">
+      <c r="M23" s="1" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="24" spans="1:13">
-      <c r="A24" s="2"/>
-      <c r="B24" s="2"/>
-      <c r="C24" s="2"/>
-      <c r="D24" s="2"/>
-      <c r="E24" s="2"/>
-      <c r="F24" s="2"/>
-      <c r="G24" s="2"/>
-      <c r="H24" s="2"/>
-      <c r="I24" s="4">
+    <row r="24" spans="9:13">
+      <c r="I24" s="1">
         <v>3</v>
       </c>
-      <c r="J24" s="4" t="s">
+      <c r="J24" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="K24" s="4">
-        <v>0</v>
-      </c>
-      <c r="L24" s="4" t="s">
+      <c r="K24" s="1">
+        <v>0</v>
+      </c>
+      <c r="L24" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="M24" s="4" t="s">
+      <c r="M24" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="25" spans="1:13">
-      <c r="A25" s="2"/>
-      <c r="B25" s="2"/>
-      <c r="C25" s="2"/>
-      <c r="D25" s="2"/>
-      <c r="E25" s="2"/>
-      <c r="F25" s="2"/>
-      <c r="G25" s="2"/>
-      <c r="H25" s="2"/>
-      <c r="I25" s="4">
+    <row r="25" spans="9:13">
+      <c r="I25" s="1">
         <v>4</v>
       </c>
-      <c r="J25" s="4" t="s">
+      <c r="J25" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="K25" s="4">
-        <v>0</v>
-      </c>
-      <c r="L25" s="4" t="s">
+      <c r="K25" s="1">
+        <v>0</v>
+      </c>
+      <c r="L25" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="M25" s="4" t="s">
+      <c r="M25" s="1" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="26" spans="1:13">
-      <c r="A26" s="2"/>
-      <c r="B26" s="2"/>
-      <c r="C26" s="2"/>
-      <c r="D26" s="2"/>
-      <c r="E26" s="2"/>
-      <c r="F26" s="2"/>
-      <c r="G26" s="2"/>
-      <c r="H26" s="2"/>
-      <c r="I26" s="4">
+    <row r="26" spans="9:13">
+      <c r="I26" s="1">
         <v>1</v>
       </c>
-      <c r="J26" s="4" t="s">
+      <c r="J26" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="K26" s="4" t="s">
+      <c r="K26" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="L26" s="4" t="s">
+      <c r="L26" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="M26" s="4" t="s">
+      <c r="M26" s="1" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="27" spans="1:13">
-      <c r="A27" s="2"/>
-      <c r="B27" s="2"/>
-      <c r="C27" s="2"/>
-      <c r="D27" s="2"/>
-      <c r="E27" s="2"/>
-      <c r="F27" s="2"/>
-      <c r="G27" s="2"/>
-      <c r="H27" s="2"/>
-      <c r="I27" s="4">
+    <row r="27" spans="9:13">
+      <c r="I27" s="1">
         <v>2</v>
       </c>
-      <c r="J27" s="4" t="s">
+      <c r="J27" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="K27" s="4" t="s">
+      <c r="K27" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="L27" s="4" t="s">
+      <c r="L27" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="M27" s="4" t="s">
+      <c r="M27" s="1" t="s">
         <v>63</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fixed control ID gen
</commit_message>
<xml_diff>
--- a/tests/data/excel/test.xlsx
+++ b/tests/data/excel/test.xlsx
@@ -143,16 +143,16 @@
     <t>XAA001LA4</t>
   </si>
   <si>
-    <t>XAA001AZ1</t>
-  </si>
-  <si>
-    <t>XAA001AZ2</t>
-  </si>
-  <si>
-    <t>XAA001AZ3</t>
-  </si>
-  <si>
-    <t>XAA001AZ4</t>
+    <t>XAA997AZ1</t>
+  </si>
+  <si>
+    <t>XAA997AZ2</t>
+  </si>
+  <si>
+    <t>XAA997AZ3</t>
+  </si>
+  <si>
+    <t>XAA997AZ4</t>
   </si>
   <si>
     <t>XAA001LB1</t>
@@ -167,16 +167,16 @@
     <t>XAA001LB4</t>
   </si>
   <si>
-    <t>XAA001BZ1</t>
-  </si>
-  <si>
-    <t>XAA001BZ2</t>
-  </si>
-  <si>
-    <t>XAA001BZ3</t>
-  </si>
-  <si>
-    <t>XAA001BZ4</t>
+    <t>XAA997BZ1</t>
+  </si>
+  <si>
+    <t>XAA997BZ2</t>
+  </si>
+  <si>
+    <t>XAA997BZ3</t>
+  </si>
+  <si>
+    <t>XAA997BZ4</t>
   </si>
   <si>
     <t>XAA001LC1</t>
@@ -191,16 +191,16 @@
     <t>XAA001LC4</t>
   </si>
   <si>
-    <t>XAA001CZ1</t>
-  </si>
-  <si>
-    <t>XAA001CZ2</t>
-  </si>
-  <si>
-    <t>XAA001CZ3</t>
-  </si>
-  <si>
-    <t>XAA001CZ4</t>
+    <t>XAA997CZ1</t>
+  </si>
+  <si>
+    <t>XAA997CZ2</t>
+  </si>
+  <si>
+    <t>XAA997CZ3</t>
+  </si>
+  <si>
+    <t>XAA997CZ4</t>
   </si>
   <si>
     <t>XAA998ZS1</t>

</xml_diff>